<commit_message>
Bildplazierung funktioniert jetzt. Ca. 36 Charaktere schon enthalten.
</commit_message>
<xml_diff>
--- a/ClashRoyaleKartendaten.xlsx
+++ b/ClashRoyaleKartendaten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Udo\Documents\github\clashroyalequartett\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4B5F63-E467-4DA3-935A-541313F5A26B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEBB7E1-E07F-4787-BE0D-DBFB44F1D1EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2352" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3528" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="158">
   <si>
     <t>Nummer</t>
   </si>
@@ -225,9 +225,6 @@
     <t>Tunnelgräber</t>
   </si>
   <si>
-    <t>Feuerwehrkerin</t>
-  </si>
-  <si>
     <t>Firecracker</t>
   </si>
   <si>
@@ -457,6 +454,51 @@
   </si>
   <si>
     <t>Barbarians</t>
+  </si>
+  <si>
+    <t>Goblin Gang</t>
+  </si>
+  <si>
+    <t>Feuerwerkerin</t>
+  </si>
+  <si>
+    <t>Fisherman</t>
+  </si>
+  <si>
+    <t>Goblin Cage</t>
+  </si>
+  <si>
+    <t>Flying Machine</t>
+  </si>
+  <si>
+    <t>Goblin Demolisher</t>
+  </si>
+  <si>
+    <t>Golden Knight</t>
+  </si>
+  <si>
+    <t>Giant</t>
+  </si>
+  <si>
+    <t>Cannon Cart</t>
+  </si>
+  <si>
+    <t>Goblin Machine</t>
+  </si>
+  <si>
+    <t>Archer Queen</t>
+  </si>
+  <si>
+    <t>Goblinstein</t>
+  </si>
+  <si>
+    <t>Goblins</t>
+  </si>
+  <si>
+    <t>Dark Prince</t>
+  </si>
+  <si>
+    <t>Executioner</t>
   </si>
 </sst>
 </file>
@@ -715,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1048386"/>
+  <dimension ref="A1:J1048184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:J101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -732,7 +774,7 @@
     <col min="10" max="10" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +844,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -834,7 +876,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -925,7 +967,9 @@
       <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>155</v>
+      </c>
       <c r="D7" s="3">
         <v>2</v>
       </c>
@@ -1262,7 +1306,7 @@
         <v>44</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
@@ -1687,7 +1731,9 @@
       <c r="B32" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="D32" s="2">
         <v>3</v>
       </c>
@@ -1837,10 +1883,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="D37" s="3">
         <v>3</v>
@@ -1869,7 +1915,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2">
@@ -1899,7 +1945,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3">
@@ -1929,7 +1975,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2">
@@ -1959,10 +2005,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="D41" s="3">
         <v>3</v>
@@ -1991,7 +2037,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2">
@@ -2021,16 +2067,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>142</v>
-      </c>
       <c r="D43" s="3">
         <v>3</v>
       </c>
       <c r="E43" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>38</v>
@@ -2053,7 +2099,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2">
@@ -2083,7 +2129,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3">
@@ -2113,14 +2159,14 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2">
         <v>3</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>35</v>
@@ -2143,9 +2189,11 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="D47" s="3">
         <v>3</v>
       </c>
@@ -2173,7 +2221,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2">
@@ -2203,7 +2251,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3">
@@ -2233,7 +2281,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2">
@@ -2263,9 +2311,11 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C51" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>146</v>
+      </c>
       <c r="D51" s="3">
         <v>4</v>
       </c>
@@ -2293,7 +2343,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2">
@@ -2323,7 +2373,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3">
@@ -2353,10 +2403,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="D54" s="2">
         <v>4</v>
@@ -2385,7 +2435,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3">
@@ -2415,7 +2465,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2">
@@ -2445,7 +2495,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3">
@@ -2475,7 +2525,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2">
@@ -2505,9 +2555,11 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C59" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>147</v>
+      </c>
       <c r="D59" s="3">
         <v>4</v>
       </c>
@@ -2569,7 +2621,9 @@
       <c r="B61" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="3"/>
+      <c r="C61" s="3" t="s">
+        <v>156</v>
+      </c>
       <c r="D61" s="3">
         <v>4</v>
       </c>
@@ -2597,10 +2651,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="D62" s="2">
         <v>4</v>
@@ -2629,7 +2683,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3">
@@ -2659,7 +2713,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2">
@@ -2689,7 +2743,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3">
@@ -2719,7 +2773,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2">
@@ -2749,7 +2803,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3">
@@ -2779,10 +2833,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="D68" s="2">
         <v>4</v>
@@ -2811,7 +2865,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3">
@@ -2841,7 +2895,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2">
@@ -2871,10 +2925,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D71" s="3">
         <v>4</v>
@@ -2903,9 +2957,11 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C72" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>148</v>
+      </c>
       <c r="D72" s="2">
         <v>4</v>
       </c>
@@ -2963,7 +3019,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2">
@@ -2993,7 +3049,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3">
@@ -3023,7 +3079,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2">
@@ -3053,7 +3109,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3">
@@ -3083,10 +3139,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D78" s="2">
         <v>4</v>
@@ -3115,9 +3171,11 @@
         <v>78</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C79" s="3"/>
+        <v>109</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>149</v>
+      </c>
       <c r="D79" s="3">
         <v>4</v>
       </c>
@@ -3137,7 +3195,7 @@
         <v>1799</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3145,7 +3203,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2">
@@ -3167,7 +3225,7 @@
         <v>2250</v>
       </c>
       <c r="J80" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3175,9 +3233,11 @@
         <v>80</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C81" s="3"/>
+        <v>112</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="D81" s="3">
         <v>5</v>
       </c>
@@ -3205,10 +3265,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D82" s="2">
         <v>5</v>
@@ -3237,7 +3297,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3">
@@ -3267,7 +3327,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2">
@@ -3297,7 +3357,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3">
@@ -3327,7 +3387,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2">
@@ -3357,10 +3417,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="D87" s="3">
         <v>5</v>
@@ -3389,7 +3449,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2">
@@ -3419,7 +3479,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="3">
@@ -3449,7 +3509,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2">
@@ -3479,10 +3539,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D91" s="3">
         <v>5</v>
@@ -3511,7 +3571,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2">
@@ -3541,7 +3601,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3">
@@ -3571,9 +3631,11 @@
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C94" s="2"/>
+        <v>131</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="D94" s="2">
         <v>5</v>
       </c>
@@ -3601,9 +3663,11 @@
         <v>94</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C95" s="3"/>
+        <v>132</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>157</v>
+      </c>
       <c r="D95" s="3">
         <v>5</v>
       </c>
@@ -3631,9 +3695,11 @@
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C96" s="2"/>
+        <v>133</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>151</v>
+      </c>
       <c r="D96" s="2">
         <v>5</v>
       </c>
@@ -3661,9 +3727,11 @@
         <v>96</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C97" s="3"/>
+        <v>134</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>152</v>
+      </c>
       <c r="D97" s="3">
         <v>5</v>
       </c>
@@ -3691,9 +3759,11 @@
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C98" s="2"/>
+        <v>135</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="D98" s="2">
         <v>5</v>
       </c>
@@ -3713,7 +3783,7 @@
         <v>1000</v>
       </c>
       <c r="J98" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="99" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3721,9 +3791,11 @@
         <v>98</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C99" s="3"/>
+        <v>136</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>154</v>
+      </c>
       <c r="D99" s="3">
         <v>5</v>
       </c>
@@ -3743,7 +3815,7 @@
         <v>2385</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3751,7 +3823,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2">
@@ -3781,7 +3853,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C101" s="3"/>
       <c r="D101" s="3">
@@ -3806,98 +3878,98 @@
         <v>22</v>
       </c>
     </row>
-    <row r="1048295" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048296" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048297" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048298" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048299" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048300" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048301" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048302" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048303" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048304" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048305" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048306" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048307" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048308" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048309" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048310" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048311" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048312" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048313" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048314" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048315" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048316" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048317" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048318" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048319" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048320" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048321" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048322" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048323" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048324" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048325" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048326" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048327" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048328" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048329" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048330" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048331" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048332" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048333" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048334" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048335" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048336" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048337" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048338" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048339" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048340" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048341" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048342" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048343" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048344" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048345" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048346" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048347" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048348" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048349" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048350" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048351" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048352" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048353" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048354" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048355" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048356" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048357" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048358" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048359" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048360" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048361" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048362" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048363" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048364" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048365" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048366" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048367" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048368" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048369" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048370" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048371" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048372" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048373" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048374" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048375" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048376" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048377" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048378" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048379" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048380" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048381" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048382" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048383" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048384" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048385" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="1048386" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048093" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048094" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048095" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048096" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048097" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048098" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048099" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048100" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048101" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048102" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048103" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048104" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048105" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048106" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048107" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048108" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048109" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048110" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048111" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048112" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048113" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048114" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048115" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048116" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048117" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048118" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048119" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048120" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048121" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048122" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048123" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048124" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048125" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048126" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048127" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048128" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048129" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048130" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048131" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048132" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048133" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048134" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048135" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048136" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048137" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048138" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048139" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048140" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048141" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048142" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048143" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048144" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048145" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048146" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048147" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048148" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048149" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048150" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048151" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048152" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048153" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048154" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048155" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048156" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048157" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048158" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048159" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048160" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048161" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048162" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048163" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048164" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048165" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048166" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048167" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048168" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048169" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048170" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048171" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048172" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048173" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048174" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048175" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048176" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048177" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048178" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048179" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048180" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048181" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048182" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048183" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="1048184" ht="14.4" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
jetzt mit 72 kartendaten
</commit_message>
<xml_diff>
--- a/ClashRoyaleKartendaten.xlsx
+++ b/ClashRoyaleKartendaten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Udo\Documents\github\clashroyalequartett\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEBB7E1-E07F-4787-BE0D-DBFB44F1D1EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F978195-55C9-449D-97C0-A1CB9965AE01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3528" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4704" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="191">
   <si>
     <t>Nummer</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Legendär</t>
   </si>
   <si>
-    <t>Skelette</t>
-  </si>
-  <si>
     <t>NK:Gering</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>Feuergeist</t>
   </si>
   <si>
-    <t>Sehr Schnell</t>
-  </si>
-  <si>
     <t>Elektrogeist</t>
   </si>
   <si>
@@ -117,9 +111,6 @@
     <t>Kobolde</t>
   </si>
   <si>
-    <t>Speerkobolde</t>
-  </si>
-  <si>
     <t>Bomber</t>
   </si>
   <si>
@@ -135,9 +126,6 @@
     <t>Unbeweglich</t>
   </si>
   <si>
-    <t>Schneball</t>
-  </si>
-  <si>
     <t>Eisgolem</t>
   </si>
   <si>
@@ -159,15 +147,6 @@
     <t>Mauerbrecher</t>
   </si>
   <si>
-    <t>Schleicherbusch</t>
-  </si>
-  <si>
-    <t>Wut</t>
-  </si>
-  <si>
-    <t>Koboldfluich</t>
-  </si>
-  <si>
     <t>Ritter</t>
   </si>
   <si>
@@ -195,12 +174,6 @@
     <t>Megalakai</t>
   </si>
   <si>
-    <t>Skelettarmee</t>
-  </si>
-  <si>
-    <t>Wächter</t>
-  </si>
-  <si>
     <t>Koboldfass</t>
   </si>
   <si>
@@ -210,9 +183,6 @@
     <t>Koboldgang</t>
   </si>
   <si>
-    <t>Skelettfass</t>
-  </si>
-  <si>
     <t>Blasrohrkobold</t>
   </si>
   <si>
@@ -222,9 +192,6 @@
     <t>Prinzessin</t>
   </si>
   <si>
-    <t>Tunnelgräber</t>
-  </si>
-  <si>
     <t>Firecracker</t>
   </si>
   <si>
@@ -246,9 +213,6 @@
     <t>Königliche Luftpost</t>
   </si>
   <si>
-    <t>Tornado</t>
-  </si>
-  <si>
     <t>Klonzauber</t>
   </si>
   <si>
@@ -264,9 +228,6 @@
     <t>Musketierin</t>
   </si>
   <si>
-    <t>MiniP.E.K.K.A.</t>
-  </si>
-  <si>
     <t>Koboldhütte</t>
   </si>
   <si>
@@ -276,30 +237,18 @@
     <t>Feuerball</t>
   </si>
   <si>
-    <t>Walküre</t>
-  </si>
-  <si>
     <t>Rammbock</t>
   </si>
   <si>
     <t>Battle Ram</t>
   </si>
   <si>
-    <t>Skelettdrachen</t>
-  </si>
-  <si>
     <t>Bomberturm</t>
   </si>
   <si>
     <t>Minenwerfer</t>
   </si>
   <si>
-    <t>Schweinereiter</t>
-  </si>
-  <si>
-    <t>Flugmaschiene</t>
-  </si>
-  <si>
     <t>Kampfheilerin</t>
   </si>
   <si>
@@ -309,18 +258,9 @@
     <t>Frost</t>
   </si>
   <si>
-    <t>Runenriesin</t>
-  </si>
-  <si>
     <t>Gift</t>
   </si>
   <si>
-    <t>Tesla</t>
-  </si>
-  <si>
-    <t>Zappys</t>
-  </si>
-  <si>
     <t>Ofen</t>
   </si>
   <si>
@@ -336,9 +276,6 @@
     <t>Elektromagier</t>
   </si>
   <si>
-    <t>Koboldfernichter</t>
-  </si>
-  <si>
     <t>Magieschütze</t>
   </si>
   <si>
@@ -393,9 +330,6 @@
     <t>Lakaieenhorde</t>
   </si>
   <si>
-    <t>Widderreiterin</t>
-  </si>
-  <si>
     <t>Elektrodrache</t>
   </si>
   <si>
@@ -405,39 +339,24 @@
     <t>Electro Spirit</t>
   </si>
   <si>
-    <t>Suspicious Bush</t>
-  </si>
-  <si>
     <t>Electro Wizard</t>
   </si>
   <si>
     <t>Mother Witch</t>
   </si>
   <si>
-    <t>Fridhof</t>
-  </si>
-  <si>
     <t>Rabauken</t>
   </si>
   <si>
     <t>Bowler</t>
   </si>
   <si>
-    <t>Scharfrichter</t>
-  </si>
-  <si>
     <t>Kanonenkarre</t>
   </si>
   <si>
-    <t>Koboldmaschiene</t>
-  </si>
-  <si>
     <t>Bogenschützenkönigin</t>
   </si>
   <si>
-    <t>DR. Frankenkobold</t>
-  </si>
-  <si>
     <t>Rakete</t>
   </si>
   <si>
@@ -498,7 +417,187 @@
     <t>Dark Prince</t>
   </si>
   <si>
-    <t>Executioner</t>
+    <t>Barbarenhütte</t>
+  </si>
+  <si>
+    <t>Sehr schnell</t>
+  </si>
+  <si>
+    <t>Blitz</t>
+  </si>
+  <si>
+    <t>Boss-Banditin</t>
+  </si>
+  <si>
+    <t>Boss Bandit</t>
+  </si>
+  <si>
+    <t>Dr. Frankenkobold</t>
+  </si>
+  <si>
+    <t>Drei Musketierinnen</t>
+  </si>
+  <si>
+    <t>Three Musketeers</t>
+  </si>
+  <si>
+    <t>Ice Spirit</t>
+  </si>
+  <si>
+    <t>Ice Golem</t>
+  </si>
+  <si>
+    <t>Ice Wizard</t>
+  </si>
+  <si>
+    <t>Elektroriese</t>
+  </si>
+  <si>
+    <t>Electro Giant</t>
+  </si>
+  <si>
+    <t>Elitebarbaren</t>
+  </si>
+  <si>
+    <t>Elite Barbarians</t>
+  </si>
+  <si>
+    <t>Elixiersammler</t>
+  </si>
+  <si>
+    <t>Flugmaschine</t>
+  </si>
+  <si>
+    <t>Friedhof</t>
+  </si>
+  <si>
+    <t>Funki</t>
+  </si>
+  <si>
+    <t>Sparky</t>
+  </si>
+  <si>
+    <t>Geisterkeiserin</t>
+  </si>
+  <si>
+    <t>Spirit Empress</t>
+  </si>
+  <si>
+    <t>Golem</t>
+  </si>
+  <si>
+    <t>Mighy Miner</t>
+  </si>
+  <si>
+    <t>Heal Spirit</t>
+  </si>
+  <si>
+    <t>Lumberjack</t>
+  </si>
+  <si>
+    <t>Inferno Dragon</t>
+  </si>
+  <si>
+    <t>Hunter</t>
+  </si>
+  <si>
+    <t>Kleiner Prinz</t>
+  </si>
+  <si>
+    <t>Little Prince</t>
+  </si>
+  <si>
+    <t>Koboldfluch</t>
+  </si>
+  <si>
+    <t>Koboldmaschine</t>
+  </si>
+  <si>
+    <t>Koboldriese</t>
+  </si>
+  <si>
+    <t>Goblin Giant</t>
+  </si>
+  <si>
+    <t>Koboldvernichter</t>
+  </si>
+  <si>
+    <t>Royal Ghost</t>
+  </si>
+  <si>
+    <t>Königsrekruten</t>
+  </si>
+  <si>
+    <t>Royal Recruits</t>
+  </si>
+  <si>
+    <t>Royal Giant</t>
+  </si>
+  <si>
+    <t>Royal Hogs</t>
+  </si>
+  <si>
+    <t>Minion Horde</t>
+  </si>
+  <si>
+    <t>Minions</t>
+  </si>
+  <si>
+    <t>Lavahund</t>
+  </si>
+  <si>
+    <t>Lava Hound</t>
+  </si>
+  <si>
+    <t>Magic Archer</t>
+  </si>
+  <si>
+    <t>Mega Minion</t>
+  </si>
+  <si>
+    <t>Megaritter</t>
+  </si>
+  <si>
+    <t>Mega Knight</t>
+  </si>
+  <si>
+    <t>Mini P.E.K.K.A.</t>
+  </si>
+  <si>
+    <t>Mönch</t>
+  </si>
+  <si>
+    <t>Monk</t>
+  </si>
+  <si>
+    <t>Musketeer</t>
+  </si>
+  <si>
+    <t>Night Witch</t>
+  </si>
+  <si>
+    <t>P.E.K.K.A.</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Prince</t>
+  </si>
+  <si>
+    <t>Princess</t>
+  </si>
+  <si>
+    <t>Rascals</t>
+  </si>
+  <si>
+    <t>Riesenskelett</t>
+  </si>
+  <si>
+    <t>Giant Skeleton</t>
+  </si>
+  <si>
+    <t>Knight</t>
   </si>
 </sst>
 </file>
@@ -808,322 +907,328 @@
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="H2" s="2">
-        <v>81</v>
+        <v>640</v>
       </c>
       <c r="I2" s="2">
-        <v>81</v>
+        <v>1679</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>124</v>
+        <v>60</v>
       </c>
       <c r="D3" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="3">
-        <v>2.5</v>
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="H3" s="3">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="I3" s="3">
-        <v>230</v>
+        <v>906</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="D4" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2.5</v>
+        <v>17</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H4" s="2">
-        <v>99</v>
+        <v>192</v>
       </c>
       <c r="I4" s="2">
-        <v>230</v>
+        <v>670</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G5" s="3">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="H5" s="3">
-        <v>110</v>
+        <v>230</v>
       </c>
       <c r="I5" s="3">
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>130</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G6" s="2">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="H6" s="2">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="I6" s="2">
-        <v>230</v>
+        <v>1164</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>155</v>
+        <v>36</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
       </c>
       <c r="E7" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="G7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="3">
+        <v>102</v>
+      </c>
+      <c r="I7" s="3">
+        <v>896</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="H7" s="3">
-        <v>120</v>
-      </c>
-      <c r="I7" s="3">
-        <v>202</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="D8" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>24</v>
+        <v>131</v>
       </c>
       <c r="G8" s="2">
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="H8" s="2">
-        <v>81</v>
+        <v>156</v>
       </c>
       <c r="I8" s="2">
-        <v>133</v>
+        <v>261</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E9" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G9" s="3">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="H9" s="3">
-        <v>225</v>
+        <v>1057</v>
       </c>
       <c r="I9" s="3">
-        <v>304</v>
+        <v>0</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="D10" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="2">
         <v>5</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="H10" s="2">
-        <v>81</v>
+        <v>225</v>
       </c>
       <c r="I10" s="2">
-        <v>81</v>
+        <v>1000</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="D11" s="3">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3">
         <v>2</v>
       </c>
-      <c r="E11" s="3">
-        <v>1</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G11" s="3">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="H11" s="3">
-        <v>192</v>
+        <v>112</v>
       </c>
       <c r="I11" s="3">
-        <v>0</v>
+        <v>304</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="D12" s="2">
         <v>2</v>
       </c>
@@ -1131,63 +1236,63 @@
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G12" s="2">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="H12" s="2">
-        <v>179</v>
+        <v>225</v>
       </c>
       <c r="I12" s="2">
-        <v>0</v>
+        <v>304</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="G13" s="3">
+        <v>6</v>
       </c>
       <c r="H13" s="3">
-        <v>84</v>
+        <v>222</v>
       </c>
       <c r="I13" s="3">
-        <v>1315</v>
+        <v>1356</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>133</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>134</v>
       </c>
       <c r="D14" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E14" s="2">
         <v>1</v>
@@ -1196,43 +1301,45 @@
         <v>12</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H14" s="2">
-        <v>102</v>
+        <v>537</v>
       </c>
       <c r="I14" s="2">
-        <v>896</v>
+        <v>2624</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="3"/>
+        <v>107</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="D15" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G15" s="3">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="H15" s="3">
-        <v>230</v>
+        <v>289</v>
       </c>
       <c r="I15" s="3">
-        <v>0</v>
+        <v>2081</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>13</v>
@@ -1240,59 +1347,63 @@
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="2"/>
+        <v>135</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="D16" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G16" s="2">
-        <v>10.1</v>
+        <v>5.5</v>
       </c>
       <c r="H16" s="2">
-        <v>268</v>
+        <v>128</v>
       </c>
       <c r="I16" s="2">
-        <v>0</v>
+        <v>2385</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D17" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E17" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
+      </c>
+      <c r="G17" s="3">
+        <v>3.5</v>
       </c>
       <c r="H17" s="3">
-        <v>350</v>
+        <v>161</v>
       </c>
       <c r="I17" s="3">
-        <v>330</v>
+        <v>1152</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>13</v>
@@ -1300,61 +1411,63 @@
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>136</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="D18" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E18" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G18" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H18" s="2">
-        <v>0</v>
+        <v>314</v>
       </c>
       <c r="I18" s="2">
-        <v>81</v>
+        <v>883</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>129</v>
+      </c>
       <c r="D19" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E19" s="3">
         <v>1</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="3">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H19" s="3">
-        <v>179</v>
+        <v>532</v>
       </c>
       <c r="I19" s="3">
-        <v>0</v>
+        <v>1440</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>13</v>
@@ -1362,439 +1475,455 @@
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="D20" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2">
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>35</v>
+        <v>131</v>
       </c>
       <c r="G20" s="2">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="H20" s="2">
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="I20" s="2">
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
+        <v>12</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3">
-        <v>3</v>
-      </c>
-      <c r="E21" s="3">
-        <v>1</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H21" s="3">
-        <v>202</v>
+        <v>84</v>
       </c>
       <c r="I21" s="3">
-        <v>1766</v>
+        <v>1315</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="D22" s="2">
         <v>3</v>
       </c>
       <c r="E22" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G22" s="2">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="H22" s="2">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="I22" s="2">
-        <v>304</v>
+        <v>688</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="D23" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E23" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G23" s="3">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="H23" s="3">
-        <v>107</v>
+        <v>192</v>
       </c>
       <c r="I23" s="3">
-        <v>230</v>
+        <v>949</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="D24" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E24" s="2">
         <v>1</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>35</v>
+        <v>131</v>
       </c>
       <c r="G24" s="2">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="H24" s="2">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="I24" s="2">
-        <v>366</v>
+        <v>230</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="D25" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="G25" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H25" s="3">
-        <v>0</v>
+        <v>234</v>
       </c>
       <c r="I25" s="3">
-        <v>529</v>
+        <v>714</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>54</v>
+        <v>142</v>
       </c>
       <c r="D26" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E26" s="2">
         <v>1</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" s="2">
-        <v>5.5</v>
+        <v>34</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="H26" s="2">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="I26" s="2">
-        <v>824</v>
+        <v>3855</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="3"/>
+        <v>143</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="D27" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E27" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H27" s="3">
-        <v>312</v>
+        <v>384</v>
       </c>
       <c r="I27" s="3">
-        <v>837</v>
+        <v>1341</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="D28" s="2">
         <v>3</v>
       </c>
       <c r="E28" s="2">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H28" s="2">
-        <v>81</v>
+        <v>253</v>
       </c>
       <c r="I28" s="2">
-        <v>81</v>
+        <v>1569</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E29" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
       </c>
       <c r="H29" s="3">
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="I29" s="3">
-        <v>337</v>
+        <v>1070</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2">
         <v>3</v>
       </c>
       <c r="E30" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G30" s="2">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="H30" s="2">
-        <v>0</v>
+        <v>283</v>
       </c>
       <c r="I30" s="2">
         <v>0</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E31" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G31" s="3">
         <v>2.5</v>
       </c>
       <c r="H31" s="3">
-        <v>153</v>
+        <v>688</v>
       </c>
       <c r="I31" s="3">
         <v>0</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>143</v>
+        <v>102</v>
       </c>
       <c r="D32" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E32" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>24</v>
+        <v>131</v>
       </c>
       <c r="G32" s="2">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="H32" s="2">
-        <v>120</v>
+        <v>207</v>
       </c>
       <c r="I32" s="2">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="3"/>
+        <v>117</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D33" s="3">
         <v>3</v>
       </c>
       <c r="E33" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G33" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H33" s="3">
-        <v>145</v>
+        <v>320</v>
       </c>
       <c r="I33" s="3">
-        <v>532</v>
+        <v>304</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="D34" s="2">
         <v>3</v>
@@ -1803,61 +1932,65 @@
         <v>1</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G34" s="2">
-        <v>6.5</v>
+        <v>17</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="H34" s="2">
-        <v>156</v>
+        <v>194</v>
       </c>
       <c r="I34" s="2">
-        <v>261</v>
+        <v>870</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="D35" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E35" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" s="3">
-        <v>9</v>
+        <v>131</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H35" s="3">
-        <v>168</v>
+        <v>81</v>
       </c>
       <c r="I35" s="3">
-        <v>261</v>
+        <v>81</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="2"/>
+        <v>146</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="D36" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E36" s="2">
         <v>1</v>
@@ -1865,106 +1998,106 @@
       <c r="F36" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>15</v>
+      <c r="G36" s="2">
+        <v>6</v>
       </c>
       <c r="H36" s="2">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="I36" s="2">
-        <v>1210</v>
+        <v>614</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>66</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="C37" s="3"/>
       <c r="D37" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E37" s="3">
         <v>1</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="G37" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H37" s="3">
-        <v>320</v>
+        <v>0</v>
       </c>
       <c r="I37" s="3">
-        <v>304</v>
+        <v>0</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2">
+        <v>4</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G38" s="2">
         <v>3</v>
       </c>
-      <c r="E38" s="2">
-        <v>1</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G38" s="2">
-        <v>3.5</v>
-      </c>
       <c r="H38" s="2">
-        <v>283</v>
+        <v>148</v>
       </c>
       <c r="I38" s="2">
         <v>0</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39" s="3"/>
+        <v>148</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>149</v>
+      </c>
       <c r="D39" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E39" s="3">
         <v>1</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="G39" s="3">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="H39" s="3">
-        <v>89</v>
+        <v>1331</v>
       </c>
       <c r="I39" s="3">
-        <v>688</v>
+        <v>1451</v>
       </c>
       <c r="J39" s="3" t="s">
         <v>19</v>
@@ -1972,29 +2105,31 @@
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="2"/>
+        <v>150</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>151</v>
+      </c>
       <c r="D40" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E40" s="2">
         <v>1</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="G40" s="2">
+        <v>5</v>
       </c>
       <c r="H40" s="2">
-        <v>261</v>
+        <v>307</v>
       </c>
       <c r="I40" s="2">
-        <v>1210</v>
+        <v>1244</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>19</v>
@@ -2002,104 +2137,104 @@
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>71</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="C41" s="3"/>
       <c r="D41" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E41" s="3">
         <v>1</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="G41" s="3">
+        <v>3.5</v>
       </c>
       <c r="H41" s="3">
-        <v>194</v>
+        <v>92</v>
       </c>
       <c r="I41" s="3">
-        <v>906</v>
+        <v>0</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C42" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="D42" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E42" s="2">
         <v>1</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G42" s="2">
-        <v>3</v>
+        <v>17</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="H42" s="2">
-        <v>437</v>
+        <v>161</v>
       </c>
       <c r="I42" s="2">
-        <v>0</v>
+        <v>1799</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
-        <v>42</v>
+        <v>115</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="D43" s="3">
+        <v>8</v>
+      </c>
+      <c r="E43" s="3">
         <v>3</v>
       </c>
-      <c r="E43" s="3">
-        <v>6</v>
-      </c>
       <c r="F43" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H43" s="3">
-        <v>253</v>
+        <v>312</v>
       </c>
       <c r="I43" s="3">
-        <v>1569</v>
+        <v>6159</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2">
@@ -2109,93 +2244,95 @@
         <v>1</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G44" s="2">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="H44" s="2">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="I44" s="2">
-        <v>0</v>
+        <v>529</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C45" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>153</v>
+      </c>
       <c r="D45" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E45" s="3">
         <v>1</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G45" s="3">
-        <v>3</v>
+        <v>17</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="H45" s="3">
-        <v>0</v>
+        <v>409</v>
       </c>
       <c r="I45" s="3">
-        <v>0</v>
+        <v>2250</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="D46" s="2">
-        <v>3</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>76</v>
+        <v>1</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>35</v>
+        <v>131</v>
       </c>
       <c r="G46" s="2">
         <v>2.5</v>
       </c>
       <c r="H46" s="2">
-        <v>340</v>
+        <v>110</v>
       </c>
       <c r="I46" s="2">
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>145</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="C47" s="3"/>
       <c r="D47" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E47" s="3">
         <v>1</v>
@@ -2203,27 +2340,29 @@
       <c r="F47" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G47" s="3" t="s">
-        <v>15</v>
+      <c r="G47" s="3">
+        <v>5.5</v>
       </c>
       <c r="H47" s="3">
-        <v>194</v>
+        <v>135</v>
       </c>
       <c r="I47" s="3">
-        <v>870</v>
+        <v>839</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C48" s="2"/>
+        <v>87</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="D48" s="2">
         <v>4</v>
       </c>
@@ -2234,26 +2373,28 @@
         <v>17</v>
       </c>
       <c r="G48" s="2">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="H48" s="2">
-        <v>217</v>
+        <v>133</v>
       </c>
       <c r="I48" s="2">
-        <v>721</v>
+        <v>529</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C49" s="3"/>
+        <v>85</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>155</v>
+      </c>
       <c r="D49" s="3">
         <v>4</v>
       </c>
@@ -2261,29 +2402,31 @@
         <v>1</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>12</v>
+        <v>131</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H49" s="3">
-        <v>755</v>
+        <v>256</v>
       </c>
       <c r="I49" s="3">
-        <v>1433</v>
+        <v>1282</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C50" s="2"/>
+        <v>81</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="D50" s="2">
         <v>4</v>
       </c>
@@ -2291,61 +2434,61 @@
         <v>1</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G50" s="2">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="H50" s="2">
-        <v>0</v>
+        <v>422</v>
       </c>
       <c r="I50" s="2">
-        <v>1180</v>
+        <v>1295</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>146</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C51" s="3"/>
       <c r="D51" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E51" s="3">
         <v>1</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G51" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H51" s="3">
-        <v>0</v>
+        <v>847</v>
       </c>
       <c r="I51" s="3">
-        <v>780</v>
+        <v>1748</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C52" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="D52" s="2">
         <v>4</v>
       </c>
@@ -2353,29 +2496,31 @@
         <v>1</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G52" s="2">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="H52" s="2">
-        <v>688</v>
+        <v>840</v>
       </c>
       <c r="I52" s="2">
-        <v>0</v>
+        <v>885</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C53" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="D53" s="3">
         <v>4</v>
       </c>
@@ -2386,212 +2531,212 @@
         <v>17</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H53" s="3">
-        <v>266</v>
+        <v>148</v>
       </c>
       <c r="I53" s="3">
-        <v>1907</v>
+        <v>1717</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>85</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C54" s="2"/>
       <c r="D54" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E54" s="2">
         <v>1</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="G54" s="2">
+        <v>10.1</v>
       </c>
       <c r="H54" s="2">
-        <v>573</v>
+        <v>268</v>
       </c>
       <c r="I54" s="2">
-        <v>967</v>
+        <v>0</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C55" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="D55" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E55" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="G55" s="3">
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="H55" s="3">
-        <v>161</v>
+        <v>212</v>
       </c>
       <c r="I55" s="3">
-        <v>560</v>
+        <v>824</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C56" s="2"/>
+        <v>108</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="D56" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E56" s="2">
         <v>1</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G56" s="2">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="H56" s="2">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="I56" s="2">
-        <v>1356</v>
+        <v>1809</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
-        <v>56</v>
+        <v>117</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C57" s="3"/>
+        <v>158</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="D57" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E57" s="3">
         <v>1</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G57" s="3">
-        <v>11.5</v>
+        <v>5.5</v>
       </c>
       <c r="H57" s="3">
-        <v>266</v>
+        <v>99</v>
       </c>
       <c r="I57" s="3">
-        <v>1369</v>
+        <v>698</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E58" s="2">
         <v>1</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="G58" s="2">
+        <v>3</v>
       </c>
       <c r="H58" s="2">
-        <v>317</v>
+        <v>0</v>
       </c>
       <c r="I58" s="2">
-        <v>1697</v>
+        <v>0</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>147</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C59" s="3"/>
       <c r="D59" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E59" s="3">
         <v>1</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="G59" s="3">
-        <v>6</v>
+        <v>2.5</v>
       </c>
       <c r="H59" s="3">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="I59" s="3">
-        <v>614</v>
+        <v>0</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="C60" s="2"/>
       <c r="D60" s="2">
         <v>4</v>
       </c>
@@ -2599,16 +2744,16 @@
         <v>1</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="G60" s="2">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="H60" s="2">
-        <v>161</v>
+        <v>84</v>
       </c>
       <c r="I60" s="2">
-        <v>1152</v>
+        <v>1313</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>13</v>
@@ -2616,90 +2761,88 @@
     </row>
     <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="D61" s="3">
+        <v>2</v>
+      </c>
+      <c r="E61" s="3">
         <v>4</v>
       </c>
-      <c r="E61" s="3">
-        <v>1</v>
-      </c>
       <c r="F61" s="3" t="s">
-        <v>12</v>
+        <v>131</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H61" s="3">
-        <v>532</v>
+        <v>120</v>
       </c>
       <c r="I61" s="3">
-        <v>1440</v>
+        <v>202</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>92</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C62" s="2"/>
       <c r="D62" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E62" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="G62" s="2">
+        <v>1.5</v>
       </c>
       <c r="H62" s="2">
-        <v>148</v>
+        <v>0</v>
       </c>
       <c r="I62" s="2">
-        <v>1717</v>
+        <v>0</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>93</v>
+        <v>160</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E63" s="3">
         <v>1</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G63" s="3">
         <v>3</v>
       </c>
       <c r="H63" s="3">
-        <v>148</v>
+        <v>35</v>
       </c>
       <c r="I63" s="3">
         <v>0</v>
@@ -2710,40 +2853,42 @@
     </row>
     <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C64" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="D64" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E64" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>15</v>
+        <v>131</v>
+      </c>
+      <c r="G64" s="2">
+        <v>5</v>
       </c>
       <c r="H64" s="2">
         <v>120</v>
       </c>
       <c r="I64" s="2">
-        <v>2662</v>
+        <v>202</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3">
@@ -2753,29 +2898,31 @@
         <v>1</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G65" s="3">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="H65" s="3">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="I65" s="3">
-        <v>0</v>
+        <v>1180</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C66" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="D66" s="2">
         <v>4</v>
       </c>
@@ -2783,63 +2930,65 @@
         <v>1</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G66" s="2">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="H66" s="2">
-        <v>220</v>
+        <v>0</v>
       </c>
       <c r="I66" s="2">
-        <v>1152</v>
+        <v>780</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C67" s="3"/>
+        <v>161</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="D67" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E67" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G67" s="3">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="H67" s="3">
-        <v>117</v>
+        <v>304</v>
       </c>
       <c r="I67" s="3">
-        <v>529</v>
+        <v>2150</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>98</v>
+        <v>162</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>99</v>
+        <v>163</v>
       </c>
       <c r="D68" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E68" s="2">
         <v>1</v>
@@ -2848,26 +2997,28 @@
         <v>17</v>
       </c>
       <c r="G68" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H68" s="2">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I68" s="2">
-        <v>727</v>
+        <v>3020</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C69" s="3"/>
+        <v>164</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="D69" s="3">
         <v>4</v>
       </c>
@@ -2878,60 +3029,60 @@
         <v>17</v>
       </c>
       <c r="G69" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H69" s="3">
-        <v>840</v>
+        <v>186</v>
       </c>
       <c r="I69" s="3">
-        <v>885</v>
+        <v>1300</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E70" s="2">
         <v>1</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G70" s="2">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="H70" s="2">
-        <v>422</v>
+        <v>437</v>
       </c>
       <c r="I70" s="2">
-        <v>1295</v>
+        <v>0</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="D71" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E71" s="3">
         <v>1</v>
@@ -2939,14 +3090,14 @@
       <c r="F71" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G71" s="3">
-        <v>5</v>
+      <c r="G71" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H71" s="3">
-        <v>234</v>
+        <v>261</v>
       </c>
       <c r="I71" s="3">
-        <v>714</v>
+        <v>1210</v>
       </c>
       <c r="J71" s="3" t="s">
         <v>19</v>
@@ -2954,181 +3105,191 @@
     </row>
     <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>103</v>
+        <v>166</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="D72" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E72" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G72" s="2">
-        <v>5</v>
+      <c r="G72" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="H72" s="2">
-        <v>186</v>
+        <v>133</v>
       </c>
       <c r="I72" s="2">
-        <v>1300</v>
+        <v>787</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C73" s="3"/>
+        <v>111</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="D73" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E73" s="3">
         <v>1</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>18</v>
+        <v>34</v>
+      </c>
+      <c r="G73" s="3">
+        <v>5</v>
       </c>
       <c r="H73" s="3">
-        <v>217</v>
+        <v>307</v>
       </c>
       <c r="I73" s="3">
-        <v>1052</v>
+        <v>3164</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C74" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>169</v>
+      </c>
       <c r="D74" s="2">
+        <v>5</v>
+      </c>
+      <c r="E74" s="2">
         <v>4</v>
       </c>
-      <c r="E74" s="2">
-        <v>1</v>
-      </c>
       <c r="F74" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G74" s="2">
-        <v>7</v>
+        <v>131</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H74" s="2">
-        <v>143</v>
+        <v>74</v>
       </c>
       <c r="I74" s="2">
-        <v>529</v>
+        <v>837</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C75" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>170</v>
+      </c>
       <c r="D75" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E75" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="G75" s="3">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="H75" s="3">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="I75" s="3">
-        <v>1313</v>
+        <v>230</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C76" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="D76" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E76" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G76" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="H76" s="2">
+        <v>107</v>
+      </c>
+      <c r="I76" s="2">
+        <v>230</v>
+      </c>
+      <c r="J76" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="H76" s="2">
-        <v>256</v>
-      </c>
-      <c r="I76" s="2">
-        <v>1282</v>
-      </c>
-      <c r="J76" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C77" s="3"/>
+        <v>172</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>173</v>
+      </c>
       <c r="D77" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E77" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G77" s="3" t="s">
-        <v>18</v>
+      <c r="G77" s="3">
+        <v>3.5</v>
       </c>
       <c r="H77" s="3">
-        <v>314</v>
+        <v>81</v>
       </c>
       <c r="I77" s="3">
-        <v>906</v>
+        <v>3581</v>
       </c>
       <c r="J77" s="3" t="s">
         <v>19</v>
@@ -3136,48 +3297,44 @@
     </row>
     <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>128</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C78" s="2"/>
       <c r="D78" s="2">
-        <v>4</v>
-      </c>
-      <c r="E78" s="2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G78" s="2">
-        <v>5.5</v>
+        <v>2.5</v>
       </c>
       <c r="H78" s="2">
-        <v>133</v>
+        <v>340</v>
       </c>
       <c r="I78" s="2">
-        <v>529</v>
+        <v>0</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>149</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="C79" s="3"/>
       <c r="D79" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E79" s="3">
         <v>1</v>
@@ -3185,27 +3342,29 @@
       <c r="F79" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G79" s="3" t="s">
-        <v>15</v>
+      <c r="G79" s="3">
+        <v>5.5</v>
       </c>
       <c r="H79" s="3">
-        <v>161</v>
+        <v>281</v>
       </c>
       <c r="I79" s="3">
-        <v>1799</v>
+        <v>755</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C80" s="2"/>
+        <v>83</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>174</v>
+      </c>
       <c r="D80" s="2">
         <v>4</v>
       </c>
@@ -3215,93 +3374,93 @@
       <c r="F80" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G80" s="2" t="s">
-        <v>18</v>
+      <c r="G80" s="2">
+        <v>7</v>
       </c>
       <c r="H80" s="2">
-        <v>409</v>
+        <v>143</v>
       </c>
       <c r="I80" s="2">
-        <v>2250</v>
+        <v>529</v>
       </c>
       <c r="J80" s="2" t="s">
-        <v>110</v>
+        <v>19</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>150</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C81" s="3"/>
       <c r="D81" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E81" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H81" s="3">
-        <v>253</v>
+        <v>350</v>
       </c>
       <c r="I81" s="3">
-        <v>4090</v>
+        <v>330</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>113</v>
+        <v>48</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>142</v>
+        <v>175</v>
       </c>
       <c r="D82" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E82" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H82" s="2">
-        <v>192</v>
+        <v>312</v>
       </c>
       <c r="I82" s="2">
-        <v>670</v>
+        <v>837</v>
       </c>
       <c r="J82" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C83" s="3"/>
+        <v>176</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="D83" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E83" s="3">
         <v>1</v>
@@ -3309,121 +3468,125 @@
       <c r="F83" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G83" s="3">
-        <v>5.5</v>
+      <c r="G83" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H83" s="3">
-        <v>281</v>
+        <v>537</v>
       </c>
       <c r="I83" s="3">
-        <v>755</v>
+        <v>3993</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>115</v>
+        <v>73</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E84" s="2">
         <v>1</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G84" s="2">
-        <v>6</v>
+        <v>11.5</v>
       </c>
       <c r="H84" s="2">
-        <v>847</v>
+        <v>266</v>
       </c>
       <c r="I84" s="2">
-        <v>1748</v>
+        <v>1369</v>
       </c>
       <c r="J84" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C85" s="3"/>
+        <v>178</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>178</v>
+      </c>
       <c r="D85" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E85" s="3">
         <v>1</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G85" s="3">
-        <v>5.5</v>
+        <v>12</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="H85" s="3">
-        <v>135</v>
+        <v>755</v>
       </c>
       <c r="I85" s="3">
-        <v>839</v>
+        <v>1433</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C86" s="2"/>
+        <v>179</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>180</v>
+      </c>
       <c r="D86" s="2">
         <v>5</v>
       </c>
       <c r="E86" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H86" s="2">
-        <v>74</v>
+        <v>422</v>
       </c>
       <c r="I86" s="2">
-        <v>837</v>
+        <v>2214</v>
       </c>
       <c r="J86" s="2" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>119</v>
+        <v>181</v>
       </c>
       <c r="D87" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E87" s="3">
         <v>1</v>
@@ -3431,29 +3594,31 @@
       <c r="F87" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G87" s="3" t="s">
-        <v>21</v>
+      <c r="G87" s="3">
+        <v>6</v>
       </c>
       <c r="H87" s="3">
-        <v>640</v>
+        <v>217</v>
       </c>
       <c r="I87" s="3">
-        <v>1679</v>
+        <v>721</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C88" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>182</v>
+      </c>
       <c r="D88" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E88" s="2">
         <v>1</v>
@@ -3465,132 +3630,136 @@
         <v>18</v>
       </c>
       <c r="H88" s="2">
-        <v>783</v>
+        <v>314</v>
       </c>
       <c r="I88" s="2">
-        <v>1920</v>
+        <v>906</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C89" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="D89" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E89" s="3">
+        <v>1</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G89" s="3">
         <v>6</v>
       </c>
-      <c r="F89" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G89" s="3">
-        <v>2.5</v>
-      </c>
       <c r="H89" s="3">
-        <v>107</v>
+        <v>179</v>
       </c>
       <c r="I89" s="3">
-        <v>230</v>
+        <v>727</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C90" s="2"/>
+        <v>183</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>183</v>
+      </c>
       <c r="D90" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E90" s="2">
         <v>1</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H90" s="2">
-        <v>501</v>
+        <v>816</v>
       </c>
       <c r="I90" s="2">
-        <v>1697</v>
+        <v>3760</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>139</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C91" s="3"/>
       <c r="D91" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E91" s="3">
         <v>1</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G91" s="3">
         <v>3.5</v>
       </c>
       <c r="H91" s="3">
-        <v>192</v>
+        <v>0</v>
       </c>
       <c r="I91" s="3">
-        <v>949</v>
+        <v>366</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C92" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>184</v>
+      </c>
       <c r="D92" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E92" s="2">
         <v>1</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G92" s="2">
-        <v>4</v>
+        <v>17</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="H92" s="2">
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="I92" s="2">
-        <v>0</v>
+        <v>1052</v>
       </c>
       <c r="J92" s="2" t="s">
         <v>19</v>
@@ -3598,142 +3767,142 @@
     </row>
     <row r="93" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C93" s="3"/>
+        <v>99</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>185</v>
+      </c>
       <c r="D93" s="3">
         <v>5</v>
       </c>
       <c r="E93" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F93" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G93" s="3">
-        <v>5</v>
+      <c r="G93" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="H93" s="3">
-        <v>217</v>
+        <v>783</v>
       </c>
       <c r="I93" s="3">
-        <v>1940</v>
+        <v>1920</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>131</v>
+        <v>54</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>131</v>
+        <v>186</v>
       </c>
       <c r="D94" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E94" s="2">
         <v>1</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="G94" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H94" s="2">
-        <v>289</v>
+        <v>168</v>
       </c>
       <c r="I94" s="2">
-        <v>2081</v>
+        <v>261</v>
       </c>
       <c r="J94" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
       <c r="D95" s="3">
         <v>5</v>
       </c>
       <c r="E95" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F95" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G95" s="3">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="H95" s="3">
-        <v>336</v>
+        <v>217</v>
       </c>
       <c r="I95" s="3">
-        <v>1280</v>
+        <v>1940</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>151</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C96" s="2"/>
       <c r="D96" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E96" s="2">
         <v>1</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G96" s="2">
-        <v>5.5</v>
+        <v>2</v>
       </c>
       <c r="H96" s="2">
-        <v>212</v>
+        <v>1484</v>
       </c>
       <c r="I96" s="2">
-        <v>1809</v>
+        <v>0</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="97" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>152</v>
+        <v>71</v>
       </c>
       <c r="D97" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E97" s="3">
         <v>1</v>
@@ -3741,60 +3910,58 @@
       <c r="F97" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G97" s="3">
-        <v>5</v>
+      <c r="G97" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="H97" s="3">
-        <v>304</v>
+        <v>573</v>
       </c>
       <c r="I97" s="3">
-        <v>2150</v>
+        <v>967</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="98" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C98" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2">
+        <v>3</v>
+      </c>
+      <c r="E98" s="2">
+        <v>3</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G98" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="H98" s="2">
         <v>153</v>
       </c>
-      <c r="D98" s="2">
-        <v>5</v>
-      </c>
-      <c r="E98" s="2">
-        <v>1</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G98" s="2">
-        <v>5</v>
-      </c>
-      <c r="H98" s="2">
-        <v>225</v>
-      </c>
       <c r="I98" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J98" s="2" t="s">
-        <v>110</v>
+        <v>13</v>
       </c>
     </row>
     <row r="99" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>136</v>
+        <v>91</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>154</v>
+        <v>123</v>
       </c>
       <c r="D99" s="3">
         <v>5</v>
@@ -3803,29 +3970,31 @@
         <v>1</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G99" s="3">
-        <v>5.5</v>
+        <v>34</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H99" s="3">
-        <v>128</v>
+        <v>253</v>
       </c>
       <c r="I99" s="3">
-        <v>2385</v>
+        <v>4090</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C100" s="2"/>
+        <v>188</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>189</v>
+      </c>
       <c r="D100" s="2">
         <v>6</v>
       </c>
@@ -3833,49 +4002,51 @@
         <v>1</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G100" s="2">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H100" s="2">
-        <v>1484</v>
+        <v>535</v>
       </c>
       <c r="I100" s="2">
-        <v>0</v>
+        <v>3617</v>
       </c>
       <c r="J100" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="101" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C101" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>190</v>
+      </c>
       <c r="D101" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E101" s="3">
         <v>1</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G101" s="3">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H101" s="3">
-        <v>307</v>
+        <v>202</v>
       </c>
       <c r="I101" s="3">
-        <v>3164</v>
+        <v>1766</v>
       </c>
       <c r="J101" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="1048093" ht="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Erste gedruckte Version. Seltenheits-Hintergrundbilder eingebaut. Charakterwertetabelle jetzt korrekt.
</commit_message>
<xml_diff>
--- a/ClashRoyaleKartendaten.xlsx
+++ b/ClashRoyaleKartendaten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Udo\Documents\github\clashroyalequartett\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07FA152B-2401-4389-96C0-472D425A04DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DC520A-7D81-45C2-9C93-D9072F278530}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1176" yWindow="0" windowWidth="14652" windowHeight="9516" xr2:uid="{B8457701-F67F-46DC-A223-F7332D5280E6}"/>
+    <workbookView xWindow="2352" yWindow="0" windowWidth="14652" windowHeight="9516" xr2:uid="{B8457701-F67F-46DC-A223-F7332D5280E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="266">
   <si>
     <t>Nummer</t>
   </si>
@@ -369,9 +369,6 @@
     <t>Mother Witch</t>
   </si>
   <si>
-    <t>Holtzfäller</t>
-  </si>
-  <si>
     <t>Lumberjack</t>
   </si>
   <si>
@@ -525,9 +522,6 @@
     <t>Royal Hogs</t>
   </si>
   <si>
-    <t>Lakaieenhorde</t>
-  </si>
-  <si>
     <t>Minion Horde</t>
   </si>
   <si>
@@ -738,9 +732,6 @@
     <t>Skeleton Barrel</t>
   </si>
   <si>
-    <t>Skelttekönig</t>
-  </si>
-  <si>
     <t>Skeleton King</t>
   </si>
   <si>
@@ -796,6 +787,42 @@
   </si>
   <si>
     <t>Zappies</t>
+  </si>
+  <si>
+    <t>Skelettkönig</t>
+  </si>
+  <si>
+    <t>Höhe</t>
+  </si>
+  <si>
+    <t>Sondereffekte(Erweiterung)</t>
+  </si>
+  <si>
+    <t>Hoch</t>
+  </si>
+  <si>
+    <t>Wenn die Anzahl des Gegners kleiner 3, verdoppelt sich Der Schaden</t>
+  </si>
+  <si>
+    <t>Gewinnt immer gegen Infernodrache und Infernoturm</t>
+  </si>
+  <si>
+    <t>Holzfäller</t>
+  </si>
+  <si>
+    <t>Wenn die Reichweite des Gegners kleiner 5,5 ist,wächst seine Anzahl um 1, sein Schaden um256 und seine Leben um 1600.</t>
+  </si>
+  <si>
+    <t>Lakaienhorde</t>
+  </si>
+  <si>
+    <t>Die Leben des Gegners verringern sich um den Schaden des Gegners</t>
+  </si>
+  <si>
+    <t>Je schneller der Gegner ist,desto  mehr wächst die Anzahl: Langsam:+1 Mittelschnell: +3 Schnell: +5 Sehr Schnell: +7</t>
+  </si>
+  <si>
+    <t>Verlangsamt karten um 1.</t>
   </si>
 </sst>
 </file>
@@ -858,11 +885,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1177,15 +1210,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F0702BD-B5A7-4821-820E-6C2D59392F49}">
-  <dimension ref="A1:J121"/>
+  <dimension ref="A1:L121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J121"/>
+      <selection sqref="A1:L121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="12" max="12" width="24.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1216,8 +1252,14 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>86</v>
       </c>
@@ -1248,8 +1290,10 @@
       <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>40</v>
       </c>
@@ -1280,8 +1324,10 @@
       <c r="J3" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>81</v>
       </c>
@@ -1312,8 +1358,10 @@
       <c r="J4" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>14</v>
       </c>
@@ -1344,8 +1392,10 @@
       <c r="J5" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>103</v>
       </c>
@@ -1376,8 +1426,10 @@
       <c r="J6" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>13</v>
       </c>
@@ -1408,8 +1460,10 @@
       <c r="J7" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>33</v>
       </c>
@@ -1440,8 +1494,10 @@
       <c r="J8" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>102</v>
       </c>
@@ -1472,8 +1528,10 @@
       <c r="J9" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>97</v>
       </c>
@@ -1504,8 +1562,12 @@
       <c r="J10" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>21</v>
       </c>
@@ -1536,8 +1598,12 @@
       <c r="J11" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>8</v>
       </c>
@@ -1568,8 +1634,10 @@
       <c r="J12" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>55</v>
       </c>
@@ -1600,8 +1668,10 @@
       <c r="J13" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>120</v>
       </c>
@@ -1632,8 +1702,12 @@
       <c r="J14" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K14" s="2"/>
+      <c r="L14" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>93</v>
       </c>
@@ -1664,8 +1738,10 @@
       <c r="J15" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>98</v>
       </c>
@@ -1696,8 +1772,10 @@
       <c r="J16" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>59</v>
       </c>
@@ -1728,8 +1806,10 @@
       <c r="J17" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>116</v>
       </c>
@@ -1760,8 +1840,10 @@
       <c r="J18" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>60</v>
       </c>
@@ -1792,8 +1874,10 @@
       <c r="J19" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>4</v>
       </c>
@@ -1824,8 +1908,10 @@
       <c r="J20" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>12</v>
       </c>
@@ -1856,8 +1942,10 @@
       <c r="J21" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>38</v>
       </c>
@@ -1888,8 +1976,10 @@
       <c r="J22" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>90</v>
       </c>
@@ -1920,8 +2010,10 @@
       <c r="J23" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>3</v>
       </c>
@@ -1952,8 +2044,10 @@
       <c r="J24" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>70</v>
       </c>
@@ -1984,8 +2078,12 @@
       <c r="J25" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K25" s="3"/>
+      <c r="L25" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>113</v>
       </c>
@@ -2016,8 +2114,10 @@
       <c r="J26" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>105</v>
       </c>
@@ -2048,8 +2148,10 @@
       <c r="J27" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>42</v>
       </c>
@@ -2080,8 +2182,10 @@
       <c r="J28" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>108</v>
       </c>
@@ -2112,8 +2216,10 @@
       <c r="J29" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>37</v>
       </c>
@@ -2144,8 +2250,10 @@
       <c r="J30" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>51</v>
       </c>
@@ -2176,8 +2284,10 @@
       <c r="J31" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>2</v>
       </c>
@@ -2208,8 +2318,10 @@
       <c r="J32" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>36</v>
       </c>
@@ -2240,8 +2352,10 @@
       <c r="J33" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>46</v>
       </c>
@@ -2272,8 +2386,10 @@
       <c r="J34" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>9</v>
       </c>
@@ -2304,8 +2420,10 @@
       <c r="J35" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>58</v>
       </c>
@@ -2336,8 +2454,10 @@
       <c r="J36" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>91</v>
       </c>
@@ -2368,8 +2488,10 @@
       <c r="J37" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>62</v>
       </c>
@@ -2400,8 +2522,10 @@
       <c r="J38" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>107</v>
       </c>
@@ -2432,8 +2556,10 @@
       <c r="J39" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>109</v>
       </c>
@@ -2464,8 +2590,10 @@
       <c r="J40" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>64</v>
       </c>
@@ -2496,8 +2624,10 @@
       <c r="J41" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>78</v>
       </c>
@@ -2528,8 +2658,10 @@
       <c r="J42" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>115</v>
       </c>
@@ -2560,8 +2692,10 @@
       <c r="J43" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>24</v>
       </c>
@@ -2592,8 +2726,10 @@
       <c r="J44" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>79</v>
       </c>
@@ -2624,8 +2760,10 @@
       <c r="J45" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>5</v>
       </c>
@@ -2656,8 +2794,10 @@
       <c r="J46" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>84</v>
       </c>
@@ -2688,8 +2828,10 @@
       <c r="J47" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>77</v>
       </c>
@@ -2720,16 +2862,18 @@
       <c r="J48" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>75</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="D49" s="3">
         <v>4</v>
@@ -2752,16 +2896,18 @@
       <c r="J49" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>69</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="D50" s="2">
         <v>4</v>
@@ -2784,16 +2930,18 @@
       <c r="J50" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>83</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="D51" s="3">
         <v>5</v>
@@ -2816,16 +2964,18 @@
       <c r="J51" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>68</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="D52" s="2">
         <v>4</v>
@@ -2848,16 +2998,18 @@
       <c r="J52" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>61</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="D53" s="3">
         <v>4</v>
@@ -2880,16 +3032,18 @@
       <c r="J53" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>15</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="D54" s="2">
         <v>2</v>
@@ -2912,16 +3066,18 @@
       <c r="J54" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>25</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="D55" s="3">
         <v>3</v>
@@ -2944,16 +3100,18 @@
       <c r="J55" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>95</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="D56" s="2">
         <v>5</v>
@@ -2976,16 +3134,18 @@
       <c r="J56" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="1:12" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>117</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="D57" s="3">
         <v>3</v>
@@ -3008,16 +3168,20 @@
       <c r="J57" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K57" s="3"/>
+      <c r="L57" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>44</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="D58" s="2">
         <v>3</v>
@@ -3040,16 +3204,18 @@
       <c r="J58" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>10</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="D59" s="3">
         <v>2</v>
@@ -3072,16 +3238,18 @@
       <c r="J59" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>74</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="D60" s="2">
         <v>4</v>
@@ -3104,16 +3272,18 @@
       <c r="J60" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>6</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="D61" s="3">
         <v>2</v>
@@ -3136,16 +3306,18 @@
       <c r="J61" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>29</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="D62" s="2">
         <v>3</v>
@@ -3168,16 +3340,18 @@
       <c r="J62" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>19</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="D63" s="3">
         <v>2</v>
@@ -3200,16 +3374,18 @@
       <c r="J63" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>31</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="D64" s="2">
         <v>3</v>
@@ -3232,16 +3408,18 @@
       <c r="J64" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>49</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="D65" s="3">
         <v>4</v>
@@ -3264,16 +3442,18 @@
       <c r="J65" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K65" s="3"/>
+      <c r="L65" s="3"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>50</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="D66" s="2">
         <v>4</v>
@@ -3296,16 +3476,18 @@
       <c r="J66" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>96</v>
       </c>
       <c r="B67" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="D67" s="3">
         <v>5</v>
@@ -3328,16 +3510,18 @@
       <c r="J67" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>104</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="D68" s="2">
         <v>6</v>
@@ -3360,16 +3544,18 @@
       <c r="J68" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>71</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="D69" s="3">
         <v>4</v>
@@ -3392,16 +3578,18 @@
       <c r="J69" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>41</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="D70" s="2">
         <v>3</v>
@@ -3424,16 +3612,18 @@
       <c r="J70" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>39</v>
       </c>
       <c r="B71" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="D71" s="3">
         <v>3</v>
@@ -3456,16 +3646,18 @@
       <c r="J71" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K71" s="3"/>
+      <c r="L71" s="3"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>111</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="D72" s="2">
         <v>7</v>
@@ -3488,16 +3680,18 @@
       <c r="J72" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>100</v>
       </c>
       <c r="B73" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D73" s="3">
         <v>6</v>
@@ -3520,16 +3714,18 @@
       <c r="J73" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>85</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="D74" s="2">
         <v>5</v>
@@ -3552,16 +3748,18 @@
       <c r="J74" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>88</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>166</v>
+        <v>262</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D75" s="3">
         <v>5</v>
@@ -3584,16 +3782,18 @@
       <c r="J75" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>22</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D76" s="2">
         <v>3</v>
@@ -3616,16 +3816,18 @@
       <c r="J76" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>114</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D77" s="3">
         <v>7</v>
@@ -3648,22 +3850,24 @@
       <c r="J77" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K77" s="3"/>
+      <c r="L77" s="3"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>45</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D78" s="2">
         <v>3</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>24</v>
@@ -3680,16 +3884,18 @@
       <c r="J78" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K78" s="2"/>
+      <c r="L78" s="2"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>82</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D79" s="3">
         <v>5</v>
@@ -3712,16 +3918,18 @@
       <c r="J79" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>73</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D80" s="2">
         <v>4</v>
@@ -3744,16 +3952,18 @@
       <c r="J80" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>16</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D81" s="3">
         <v>2</v>
@@ -3776,16 +3986,18 @@
       <c r="J81" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K81" s="3"/>
+      <c r="L81" s="3"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>26</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D82" s="2">
         <v>3</v>
@@ -3808,16 +4020,18 @@
       <c r="J82" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K82" s="2"/>
+      <c r="L82" s="2"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>112</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D83" s="3">
         <v>7</v>
@@ -3840,16 +4054,18 @@
       <c r="J83" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>56</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D84" s="2">
         <v>4</v>
@@ -3872,16 +4088,18 @@
       <c r="J84" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K84" s="2"/>
+      <c r="L84" s="2"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>48</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D85" s="3">
         <v>4</v>
@@ -3904,16 +4122,18 @@
       <c r="J85" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K85" s="3"/>
+      <c r="L85" s="3"/>
+    </row>
+    <row r="86" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>119</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D86" s="2">
         <v>5</v>
@@ -3936,16 +4156,20 @@
       <c r="J86" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K86" s="2"/>
+      <c r="L86" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>47</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D87" s="3">
         <v>4</v>
@@ -3968,16 +4192,18 @@
       <c r="J87" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K87" s="3"/>
+      <c r="L87" s="3"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>76</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D88" s="2">
         <v>4</v>
@@ -4000,16 +4226,18 @@
       <c r="J88" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K88" s="2"/>
+      <c r="L88" s="2"/>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>67</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D89" s="3">
         <v>4</v>
@@ -4032,16 +4260,18 @@
       <c r="J89" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K89" s="3"/>
+      <c r="L89" s="3"/>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>110</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D90" s="2">
         <v>7</v>
@@ -4064,16 +4294,18 @@
       <c r="J90" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K90" s="2"/>
+      <c r="L90" s="2"/>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>23</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D91" s="3">
         <v>3</v>
@@ -4096,16 +4328,18 @@
       <c r="J91" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>72</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D92" s="2">
         <v>4</v>
@@ -4128,16 +4362,18 @@
       <c r="J92" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K92" s="2"/>
+      <c r="L92" s="2"/>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>87</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D93" s="3">
         <v>5</v>
@@ -4160,16 +4396,18 @@
       <c r="J93" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K93" s="3"/>
+      <c r="L93" s="3"/>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>34</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D94" s="2">
         <v>3</v>
@@ -4192,16 +4430,18 @@
       <c r="J94" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K94" s="2"/>
+      <c r="L94" s="2"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>92</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D95" s="3">
         <v>5</v>
@@ -4224,16 +4464,18 @@
       <c r="J95" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K95" s="3"/>
+      <c r="L95" s="3"/>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>99</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D96" s="2">
         <v>6</v>
@@ -4256,16 +4498,18 @@
       <c r="J96" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K96" s="2"/>
+      <c r="L96" s="2"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>53</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D97" s="3">
         <v>4</v>
@@ -4288,16 +4532,18 @@
       <c r="J97" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K97" s="3"/>
+      <c r="L97" s="3"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>30</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D98" s="2">
         <v>3</v>
@@ -4320,16 +4566,18 @@
       <c r="J98" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K98" s="2"/>
+      <c r="L98" s="2"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>80</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D99" s="3">
         <v>5</v>
@@ -4352,16 +4600,18 @@
       <c r="J99" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K99" s="3"/>
+      <c r="L99" s="3"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>101</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D100" s="2">
         <v>6</v>
@@ -4384,16 +4634,18 @@
       <c r="J100" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K100" s="2"/>
+      <c r="L100" s="2"/>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>20</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D101" s="3">
         <v>3</v>
@@ -4416,16 +4668,18 @@
       <c r="J101" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K101" s="3"/>
+      <c r="L101" s="3"/>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>63</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D102" s="2">
         <v>4</v>
@@ -4448,16 +4702,18 @@
       <c r="J102" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K102" s="2"/>
+      <c r="L102" s="2"/>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>94</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D103" s="3">
         <v>5</v>
@@ -4480,16 +4736,18 @@
       <c r="J103" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K103" s="3"/>
+      <c r="L103" s="3"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>17</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D104" s="2">
         <v>2</v>
@@ -4512,16 +4770,18 @@
       <c r="J104" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K104" s="2"/>
+      <c r="L104" s="2"/>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>11</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D105" s="3">
         <v>2</v>
@@ -4544,16 +4804,18 @@
       <c r="J105" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K105" s="3"/>
+      <c r="L105" s="3"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>57</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D106" s="2">
         <v>4</v>
@@ -4576,16 +4838,18 @@
       <c r="J106" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K106" s="2"/>
+      <c r="L106" s="2"/>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>27</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D107" s="3">
         <v>3</v>
@@ -4608,16 +4872,18 @@
       <c r="J107" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K107" s="3"/>
+      <c r="L107" s="3"/>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>54</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D108" s="2">
         <v>4</v>
@@ -4640,16 +4906,18 @@
       <c r="J108" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K108" s="2"/>
+      <c r="L108" s="2"/>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>1</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D109" s="3">
         <v>1</v>
@@ -4672,16 +4940,18 @@
       <c r="J109" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K109" s="3"/>
+      <c r="L109" s="3"/>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>32</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D110" s="2">
         <v>3</v>
@@ -4704,16 +4974,18 @@
       <c r="J110" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K110" s="2"/>
+      <c r="L110" s="2"/>
+    </row>
+    <row r="111" spans="1:12" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>118</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>237</v>
+        <v>254</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D111" s="3">
         <v>4</v>
@@ -4736,16 +5008,22 @@
       <c r="J111" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K111" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L111" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>7</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D112" s="2">
         <v>2</v>
@@ -4768,16 +5046,20 @@
       <c r="J112" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K112" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L112" s="2"/>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>65</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D113" s="3">
         <v>4</v>
@@ -4800,16 +5082,20 @@
       <c r="J113" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K113" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L113" s="3"/>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>43</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D114" s="2">
         <v>3</v>
@@ -4832,16 +5118,20 @@
       <c r="J114" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K114" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L114" s="2"/>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>35</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D115" s="3">
         <v>3</v>
@@ -4864,16 +5154,20 @@
       <c r="J115" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K115" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L115" s="3"/>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>28</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D116" s="2">
         <v>3</v>
@@ -4896,16 +5190,20 @@
       <c r="J116" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K116" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L116" s="2"/>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>52</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D117" s="3">
         <v>4</v>
@@ -4928,16 +5226,20 @@
       <c r="J117" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K117" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L117" s="3"/>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>89</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D118" s="2">
         <v>5</v>
@@ -4960,16 +5262,22 @@
       <c r="J118" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K118" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L118" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>18</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D119" s="3">
         <v>2</v>
@@ -4992,16 +5300,20 @@
       <c r="J119" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K119" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L119" s="3"/>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <v>106</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D120" s="2">
         <v>6</v>
@@ -5024,16 +5336,20 @@
       <c r="J120" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K120" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L120" s="2"/>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>66</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D121" s="3">
         <v>4</v>
@@ -5056,6 +5372,10 @@
       <c r="J121" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="K121" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L121" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>